<commit_message>
Hotfix fix test about excel_parse
</commit_message>
<xml_diff>
--- a/spec/factories/data/list.xlsx
+++ b/spec/factories/data/list.xlsx
@@ -33,6 +33,21 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">手机</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="10"/>
+      </rPr>
+      <t xml:space="preserve">(phone)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">邮箱</t>
     </r>
     <r>
@@ -44,21 +59,6 @@
         <sz val="10"/>
       </rPr>
       <t xml:space="preserve">(email)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">手机</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-        <sz val="10"/>
-      </rPr>
-      <t xml:space="preserve">(phone)</t>
     </r>
   </si>
   <si>
@@ -188,7 +188,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C1" activeCellId="0" pane="topLeft" sqref="C1:C4"/>
+      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -196,7 +196,7 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="17.1326530612245"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -211,33 +211,33 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="0" t="n">
+        <v>18600000000</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>18600000000</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="0" t="n">
+        <v>18600000001</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>18600000001</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="0" t="n">
+        <v>18600000002</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>18600000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>